<commit_message>
Allow rezizing and solve multiple related issues..
</commit_message>
<xml_diff>
--- a/doc/decibel fct.xlsx
+++ b/doc/decibel fct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Java\Eclipse workspace\yavumeter\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24668B91-AA88-4906-8C12-6FC8A237828F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C61109-911A-479F-BF7B-8386EE3BC4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2440CB25-3F79-4E80-B364-14F6B0C6A509}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2440CB25-3F79-4E80-B364-14F6B0C6A509}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -4489,16 +4489,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7348CFA2-03A9-4CE0-BF59-FF92CBDA9D33}">
   <dimension ref="A3:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="18" width="6.5703125" customWidth="1"/>
+    <col min="2" max="18" width="6.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>0</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B4">
         <f t="shared" ref="B4:J4" si="1">B5*$R3/$R5</f>
         <v>0</v>
@@ -4637,7 +4637,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -4710,8 +4710,8 @@
         <v>2.1105897102992488</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="92.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="92.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>0</v>
       </c>
@@ -4780,77 +4780,77 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B9">
-        <f>B10/$R10*$R8</f>
+        <f t="shared" ref="B9:R9" si="5">B10/$R10*$R8</f>
         <v>3.292427996982291E-54</v>
       </c>
       <c r="C9">
-        <f>C10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>9.8145895343641608E-51</v>
       </c>
       <c r="D9">
-        <f>D10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>2.9256879061999001E-47</v>
       </c>
       <c r="E9">
-        <f>E10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>8.7213527315779839E-44</v>
       </c>
       <c r="F9">
-        <f>F10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>2.5997986083005584E-40</v>
       </c>
       <c r="G9">
-        <f>G10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>7.7498904261135178E-37</v>
       </c>
       <c r="H9">
-        <f>H10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>2.3102097764421319E-33</v>
       </c>
       <c r="I9">
-        <f>I10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>6.886638284827057E-30</v>
       </c>
       <c r="J9">
-        <f>J10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>2.0528779399022568E-26</v>
       </c>
       <c r="K9">
-        <f>K10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>6.1195428913734013E-23</v>
       </c>
       <c r="L9">
-        <f>L10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>1.8242100259083972E-19</v>
       </c>
       <c r="M9">
-        <f>M10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>5.4378934467732347E-16</v>
       </c>
       <c r="N9">
-        <f>N10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>1.6210131902840547E-12</v>
       </c>
       <c r="O9">
-        <f>O10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>4.8321722166772459E-9</v>
       </c>
       <c r="P9">
-        <f>P10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>1.4404502364065169E-5</v>
       </c>
       <c r="Q9">
-        <f>Q10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>4.2939216371521517E-2</v>
       </c>
       <c r="R9">
-        <f>R10/$R10*$R8</f>
+        <f t="shared" si="5"/>
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -4859,72 +4859,72 @@
         <v>2.7182818284590451</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:R10" si="5">EXP(C$3+1)</f>
+        <f t="shared" ref="C10:R10" si="6">EXP(C$3+1)</f>
         <v>8103.0839275753842</v>
       </c>
       <c r="D10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24154952.753575299</v>
       </c>
       <c r="E10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>72004899337.38588</v>
       </c>
       <c r="F10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>214643579785916.06</v>
       </c>
       <c r="G10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.3984349353005491E+17</v>
       </c>
       <c r="H10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.9073465724950998E+21</v>
       </c>
       <c r="I10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.685719999335932E+24</v>
       </c>
       <c r="J10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6948892444103338E+28</v>
       </c>
       <c r="K10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.0523936302761039E+31</v>
       </c>
       <c r="L10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5060973145850306E+35</v>
       </c>
       <c r="M10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.4896128191743455E+38</v>
       </c>
       <c r="N10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.3383347192042695E+42</v>
       </c>
       <c r="O10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.9895195705472159E+45</v>
       </c>
       <c r="P10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.1892590228282009E+49</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.5451311827611664E+52</v>
       </c>
       <c r="R10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0567887114362587E+56</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="74.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="74.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>0</v>
       </c>
@@ -4933,59 +4933,59 @@
         <v>8</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:Q12" si="6">C12+8</f>
+        <f t="shared" ref="D12:Q12" si="7">C12+8</f>
         <v>16</v>
       </c>
       <c r="E12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="F12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
       <c r="G12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="H12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="I12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>56</v>
       </c>
       <c r="J12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>64</v>
       </c>
       <c r="K12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>72</v>
       </c>
       <c r="L12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>80</v>
       </c>
       <c r="M12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>88</v>
       </c>
       <c r="N12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>96</v>
       </c>
       <c r="O12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
       <c r="P12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>112</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>120</v>
       </c>
       <c r="R12">
@@ -4993,77 +4993,77 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B13">
-        <f>B14/$R14*$R12</f>
+        <f t="shared" ref="B13:R13" si="8">B14/$R14*$R12</f>
         <v>0</v>
       </c>
       <c r="C13">
-        <f>C14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="D13">
-        <f>D14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="E13">
-        <f>E14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>4.5</v>
       </c>
       <c r="F13">
-        <f>F14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="G13">
-        <f>G14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>12.5</v>
       </c>
       <c r="H13">
-        <f>H14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="I13">
-        <f>I14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>24.5</v>
       </c>
       <c r="J13">
-        <f>J14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>32</v>
       </c>
       <c r="K13">
-        <f>K14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>40.5</v>
       </c>
       <c r="L13">
-        <f>L14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="M13">
-        <f>M14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>60.5</v>
       </c>
       <c r="N13">
-        <f>N14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>72</v>
       </c>
       <c r="O13">
-        <f>O14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>84.5</v>
       </c>
       <c r="P13">
-        <f>P14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>98</v>
       </c>
       <c r="Q13">
-        <f>Q14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>112.5</v>
       </c>
       <c r="R13">
-        <f>R14/$R14*$R12</f>
+        <f t="shared" si="8"/>
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -5072,72 +5072,72 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:R14" si="7">C$3*C$3</f>
+        <f t="shared" ref="C14:R14" si="9">C$3*C$3</f>
         <v>64</v>
       </c>
       <c r="D14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>256</v>
       </c>
       <c r="E14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>576</v>
       </c>
       <c r="F14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1024</v>
       </c>
       <c r="G14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1600</v>
       </c>
       <c r="H14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2304</v>
       </c>
       <c r="I14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3136</v>
       </c>
       <c r="J14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="K14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5184</v>
       </c>
       <c r="L14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6400</v>
       </c>
       <c r="M14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7744</v>
       </c>
       <c r="N14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>9216</v>
       </c>
       <c r="O14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>10816</v>
       </c>
       <c r="P14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>12544</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>14400</v>
       </c>
       <c r="R14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>16384</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="114.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="114.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>0</v>
       </c>
@@ -5146,59 +5146,59 @@
         <v>8</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17:Q17" si="8">C17+8</f>
+        <f t="shared" ref="D17:Q17" si="10">C17+8</f>
         <v>16</v>
       </c>
       <c r="E17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
       <c r="F17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>32</v>
       </c>
       <c r="G17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="H17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>48</v>
       </c>
       <c r="I17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>56</v>
       </c>
       <c r="J17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="K17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>72</v>
       </c>
       <c r="L17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>80</v>
       </c>
       <c r="M17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>88</v>
       </c>
       <c r="N17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>96</v>
       </c>
       <c r="O17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>104</v>
       </c>
       <c r="P17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>112</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>120</v>
       </c>
       <c r="R17">
@@ -5206,77 +5206,77 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B18">
-        <f>B19/$R19*$R17</f>
+        <f t="shared" ref="B18:R18" si="11">B19/$R19*$R17</f>
         <v>0</v>
       </c>
       <c r="C18">
-        <f>C19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>32</v>
       </c>
       <c r="D18">
-        <f>D19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>45.254833995939038</v>
       </c>
       <c r="E18">
-        <f>E19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>55.425625842204063</v>
       </c>
       <c r="F18">
-        <f>F19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>64</v>
       </c>
       <c r="G18">
-        <f>G19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>71.554175279993274</v>
       </c>
       <c r="H18">
-        <f>H19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>78.383671769061692</v>
       </c>
       <c r="I18">
-        <f>I19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>84.664041954066889</v>
       </c>
       <c r="J18">
-        <f>J19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>90.509667991878075</v>
       </c>
       <c r="K18">
-        <f>K19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>95.999999999999986</v>
       </c>
       <c r="L18">
-        <f>L19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>101.19288512538813</v>
       </c>
       <c r="M18">
-        <f>M19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>106.13199329137279</v>
       </c>
       <c r="N18">
-        <f>N19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>110.85125168440813</v>
       </c>
       <c r="O18">
-        <f>O19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>115.37764081484764</v>
       </c>
       <c r="P18">
-        <f>P19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>119.73303637676612</v>
       </c>
       <c r="Q18">
-        <f>Q19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>123.93546707863733</v>
       </c>
       <c r="R18">
-        <f>R19/$R19*$R17</f>
+        <f t="shared" si="11"/>
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -5285,71 +5285,71 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:R19" si="9">SQRT(C$3)</f>
+        <f t="shared" ref="C19:R19" si="12">SQRT(C$3)</f>
         <v>2.8284271247461903</v>
       </c>
       <c r="D19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="E19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>4.8989794855663558</v>
       </c>
       <c r="F19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>5.6568542494923806</v>
       </c>
       <c r="G19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>6.324555320336759</v>
       </c>
       <c r="H19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>6.9282032302755088</v>
       </c>
       <c r="I19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>7.4833147735478827</v>
       </c>
       <c r="J19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="K19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>8.4852813742385695</v>
       </c>
       <c r="L19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>8.9442719099991592</v>
       </c>
       <c r="M19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>9.3808315196468595</v>
       </c>
       <c r="N19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>9.7979589711327115</v>
       </c>
       <c r="O19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>10.198039027185569</v>
       </c>
       <c r="P19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>10.583005244258363</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>10.954451150103322</v>
       </c>
       <c r="R19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>11.313708498984761</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="132" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:18" ht="132" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>